<commit_message>
Fixed sprite pivots, and added class specific sprites, added to character select menu too
</commit_message>
<xml_diff>
--- a/Docs/Design/Items.xlsx
+++ b/Docs/Design/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PerForce\GradProject\Docs\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92276AF2-6695-4130-B018-0103468406AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6968C65-AB61-4F4D-947F-BF3A5AC2600C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1F875D39-1F7C-4177-96F6-BC91E1C5A10A}"/>
   </bookViews>
@@ -443,7 +443,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -462,7 +462,6 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -809,7 +808,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +888,7 @@
       <c r="F2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="18"/>
+      <c r="G2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="O2" s="12"/>
@@ -913,7 +912,7 @@
       <c r="F3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="18"/>
+      <c r="G3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
@@ -940,7 +939,7 @@
       <c r="F4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="18"/>
+      <c r="G4" s="12"/>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
@@ -1079,6 +1078,7 @@
         <v>26</v>
       </c>
       <c r="G10" s="12"/>
+      <c r="H10" s="11"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="M10" s="12"/>

</xml_diff>

<commit_message>
renamed basicattackitem and basicrangedattackitem to follow naming convention
Now called:
Weapon_MeleeAttackBasic
Weapon_RangedAttackFireBall
</commit_message>
<xml_diff>
--- a/Docs/Design/Items.xlsx
+++ b/Docs/Design/Items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Plugg\Unreal\GraduationProject\Docs\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GameProjects\Unreal\GraduationProject\Docs\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F235BC-CD25-428B-8FFA-C34A6EC6EC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8EA5C6-DE27-4E7E-976F-517DEECB3C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1F875D39-1F7C-4177-96F6-BC91E1C5A10A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1F875D39-1F7C-4177-96F6-BC91E1C5A10A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>Strike</t>
   </si>
   <si>
-    <t>BasicAttackItem</t>
-  </si>
-  <si>
     <t>Strike a target within one square for two damage.</t>
   </si>
   <si>
@@ -104,18 +101,12 @@
     <t>Fireball</t>
   </si>
   <si>
-    <t>BasicRangedAttackItem</t>
-  </si>
-  <si>
     <t>Blast a unit within a few tiles.</t>
   </si>
   <si>
     <t>Swift Shot</t>
   </si>
   <si>
-    <t>Weapon_BasicRangedBow</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -261,13 +252,22 @@
   </si>
   <si>
     <t>Is Implemented</t>
+  </si>
+  <si>
+    <t>Weapon_MeleeAttackBasic</t>
+  </si>
+  <si>
+    <t>Weapon_RangedAttackFireBall</t>
+  </si>
+  <si>
+    <t>Weapon_RangedAttackBow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,9 +464,9 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Beräkning" xfId="4" builtinId="22"/>
+    <cellStyle name="Bra" xfId="1" builtinId="26"/>
+    <cellStyle name="Dålig" xfId="2" builtinId="27"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -489,7 +489,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -808,21 +808,21 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.75" customWidth="1"/>
+    <col min="2" max="2" width="32.75" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="7" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.375" customWidth="1"/>
+    <col min="5" max="5" width="18.125" customWidth="1"/>
+    <col min="6" max="7" width="17.25" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -833,7 +833,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -842,10 +842,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>4</v>
@@ -869,48 +869,48 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="O2" s="12"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="12"/>
       <c r="J3" s="12"/>
@@ -920,345 +920,345 @@
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="12"/>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
       <c r="D5" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G5" s="11"/>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="12"/>
       <c r="K6" s="12"/>
       <c r="N6" s="12"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G7" s="12"/>
       <c r="K7" s="12"/>
       <c r="O7" s="12"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="12"/>
       <c r="K9" s="12"/>
       <c r="O9" s="12"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>50</v>
-      </c>
       <c r="F11" s="16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G11" s="12"/>
       <c r="J11" s="12"/>
       <c r="N11" s="12"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>73</v>
-      </c>
       <c r="E12" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G12" s="12"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G13" s="12"/>
       <c r="J13" s="12"/>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>57</v>
-      </c>
       <c r="E14" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G14" s="11"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="O14" s="12"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G15" s="11"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G16" s="11"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G17" s="11"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="N17" s="12"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G18" s="11"/>
       <c r="O18" s="12"/>

</xml_diff>

<commit_message>
updated excel with recent changes
</commit_message>
<xml_diff>
--- a/Docs/Design/Items.xlsx
+++ b/Docs/Design/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GameProjects\Unreal\GraduationProject\Docs\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8EA5C6-DE27-4E7E-976F-517DEECB3C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19129C4B-8E02-4B19-A58C-A2DABEE9C046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1F875D39-1F7C-4177-96F6-BC91E1C5A10A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
   <si>
     <t>Item Name</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>Weapon_RangedAttackBow</t>
+  </si>
+  <si>
+    <t>sort of</t>
   </si>
 </sst>
 </file>
@@ -808,7 +811,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -956,13 +959,13 @@
       <c r="D5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="11"/>
+      <c r="E5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="12"/>
       <c r="N5" s="12"/>
     </row>
     <row r="6" spans="1:15">

</xml_diff>

<commit_message>
Chain Lightning action and item created
</commit_message>
<xml_diff>
--- a/Docs/Design/Items.xlsx
+++ b/Docs/Design/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Plugg\Unreal\GraduationProject\Docs\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9C38D6-2D06-41FF-9B80-6E3F6950ECFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2525EAF-8406-4C68-A3C7-451CFA7934A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1F875D39-1F7C-4177-96F6-BC91E1C5A10A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
   <si>
     <t>Item Name</t>
   </si>
@@ -264,6 +264,15 @@
   </si>
   <si>
     <t>sort of</t>
+  </si>
+  <si>
+    <t>Chain Lightning</t>
+  </si>
+  <si>
+    <t>Weapon_ChainLightning</t>
+  </si>
+  <si>
+    <t>Shoot a beam of lightning at a unit, that bounces onto nearby enemies.</t>
   </si>
 </sst>
 </file>
@@ -808,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6284BC89-5930-4E5D-966B-C20FEA8FD62C}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,6 +1275,29 @@
       <c r="G18" s="11"/>
       <c r="O18" s="12"/>
     </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>